<commit_message>
Meters GUI section added
</commit_message>
<xml_diff>
--- a/downloads/Consumos medidos 2024-02 2024-02.xlsx
+++ b/downloads/Consumos medidos 2024-02 2024-02.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="60">
   <si>
     <t>Unidad kWh</t>
   </si>
@@ -187,6 +187,9 @@
   </si>
   <si>
     <t>28/02/2024</t>
+  </si>
+  <si>
+    <t>29/02/2024</t>
   </si>
   <si>
     <t>Unidad kVARh</t>
@@ -596,10 +599,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:AA30"/>
+  <dimension ref="A1:AA31"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A3" sqref="A3:A30"/>
+      <selection activeCell="A3" sqref="A3:A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2974,76 +2977,159 @@
         <v>703.81</v>
       </c>
       <c r="D30" s="3">
-        <v>145.48</v>
+        <v>606.64</v>
       </c>
       <c r="E30" s="3">
-        <v>0.0</v>
+        <v>609.5</v>
       </c>
       <c r="F30" s="3">
-        <v>0.0</v>
+        <v>605.49</v>
       </c>
       <c r="G30" s="3">
-        <v>0.0</v>
+        <v>645.74</v>
       </c>
       <c r="H30" s="3">
-        <v>0.0</v>
+        <v>839.51</v>
       </c>
       <c r="I30" s="3">
-        <v>0.0</v>
+        <v>1462.81</v>
       </c>
       <c r="J30" s="3">
-        <v>0.0</v>
+        <v>1787.68</v>
       </c>
       <c r="K30" s="3">
-        <v>0.0</v>
+        <v>1932.58</v>
       </c>
       <c r="L30" s="3">
-        <v>0.0</v>
+        <v>1981.45</v>
       </c>
       <c r="M30" s="3">
-        <v>0.0</v>
+        <v>1749.17</v>
       </c>
       <c r="N30" s="3">
-        <v>0.0</v>
+        <v>1753.76</v>
       </c>
       <c r="O30" s="3">
-        <v>0.0</v>
+        <v>2015.39</v>
       </c>
       <c r="P30" s="3">
-        <v>0.0</v>
+        <v>2042.41</v>
       </c>
       <c r="Q30" s="3">
-        <v>0.0</v>
+        <v>1919.93</v>
       </c>
       <c r="R30" s="3">
-        <v>0.0</v>
+        <v>1673.84</v>
       </c>
       <c r="S30" s="3">
-        <v>0.0</v>
+        <v>1252.36</v>
       </c>
       <c r="T30" s="3">
-        <v>0.0</v>
+        <v>1096.53</v>
       </c>
       <c r="U30" s="3">
-        <v>0.0</v>
+        <v>844.68</v>
       </c>
       <c r="V30" s="3">
-        <v>0.0</v>
+        <v>1039.61</v>
       </c>
       <c r="W30" s="3">
-        <v>0.0</v>
+        <v>1083.31</v>
       </c>
       <c r="X30" s="3">
-        <v>0.0</v>
+        <v>901.6</v>
       </c>
       <c r="Y30" s="3">
-        <v>0.0</v>
+        <v>873.43</v>
       </c>
       <c r="Z30" s="3">
-        <v>0.0</v>
+        <v>841.24</v>
       </c>
       <c r="AA30" s="3">
-        <v>849.29</v>
+        <v>30262.47</v>
+      </c>
+    </row>
+    <row r="31" spans="1:27">
+      <c r="A31" s="4">
+        <v>11002006</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C31" s="3">
+        <v>690.59</v>
+      </c>
+      <c r="D31" s="3">
+        <v>596.29</v>
+      </c>
+      <c r="E31" s="3">
+        <v>702.08</v>
+      </c>
+      <c r="F31" s="3">
+        <v>768.21</v>
+      </c>
+      <c r="G31" s="3">
+        <v>779.71</v>
+      </c>
+      <c r="H31" s="3">
+        <v>933.82</v>
+      </c>
+      <c r="I31" s="3">
+        <v>1492.71</v>
+      </c>
+      <c r="J31" s="3">
+        <v>1907.86</v>
+      </c>
+      <c r="K31" s="3">
+        <v>2042.41</v>
+      </c>
+      <c r="L31" s="3">
+        <v>2068.86</v>
+      </c>
+      <c r="M31" s="3">
+        <v>1801.48</v>
+      </c>
+      <c r="N31" s="3">
+        <v>1784.24</v>
+      </c>
+      <c r="O31" s="3">
+        <v>1980.31</v>
+      </c>
+      <c r="P31" s="3">
+        <v>2036.08</v>
+      </c>
+      <c r="Q31" s="3">
+        <v>1872.22</v>
+      </c>
+      <c r="R31" s="3">
+        <v>1587.58</v>
+      </c>
+      <c r="S31" s="3">
+        <v>1099.98</v>
+      </c>
+      <c r="T31" s="3">
+        <v>1001.09</v>
+      </c>
+      <c r="U31" s="3">
+        <v>852.16</v>
+      </c>
+      <c r="V31" s="3">
+        <v>1075.26</v>
+      </c>
+      <c r="W31" s="3">
+        <v>1091.94</v>
+      </c>
+      <c r="X31" s="3">
+        <v>914.84</v>
+      </c>
+      <c r="Y31" s="3">
+        <v>847.55</v>
+      </c>
+      <c r="Z31" s="3">
+        <v>924.04</v>
+      </c>
+      <c r="AA31" s="3">
+        <v>30851.31</v>
       </c>
     </row>
   </sheetData>
@@ -3070,10 +3156,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:AA30"/>
+  <dimension ref="A1:AA31"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A3" sqref="A3:A30"/>
+      <selection activeCell="A3" sqref="A3:A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3084,7 +3170,7 @@
   <sheetData>
     <row r="1" spans="1:27">
       <c r="A1" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -5448,76 +5534,159 @@
         <v>204.71</v>
       </c>
       <c r="D30" s="3">
-        <v>28.18</v>
+        <v>112.72</v>
       </c>
       <c r="E30" s="3">
-        <v>0.0</v>
+        <v>116.73</v>
       </c>
       <c r="F30" s="3">
-        <v>0.0</v>
+        <v>135.72</v>
       </c>
       <c r="G30" s="3">
-        <v>0.0</v>
+        <v>161.59</v>
       </c>
       <c r="H30" s="3">
-        <v>0.0</v>
+        <v>224.26</v>
       </c>
       <c r="I30" s="3">
-        <v>0.0</v>
+        <v>548.56</v>
       </c>
       <c r="J30" s="3">
-        <v>0.0</v>
+        <v>700.94</v>
       </c>
       <c r="K30" s="3">
-        <v>0.0</v>
+        <v>796.38</v>
       </c>
       <c r="L30" s="3">
-        <v>0.0</v>
+        <v>908.52</v>
       </c>
       <c r="M30" s="3">
-        <v>0.0</v>
+        <v>669.31</v>
       </c>
       <c r="N30" s="3">
-        <v>0.0</v>
+        <v>662.41</v>
       </c>
       <c r="O30" s="3">
-        <v>0.0</v>
+        <v>902.18</v>
       </c>
       <c r="P30" s="3">
-        <v>0.0</v>
+        <v>927.48</v>
       </c>
       <c r="Q30" s="3">
-        <v>0.0</v>
+        <v>779.14</v>
       </c>
       <c r="R30" s="3">
-        <v>0.0</v>
+        <v>608.36</v>
       </c>
       <c r="S30" s="3">
-        <v>0.0</v>
+        <v>443.92</v>
       </c>
       <c r="T30" s="3">
-        <v>0.0</v>
+        <v>392.17</v>
       </c>
       <c r="U30" s="3">
-        <v>0.0</v>
+        <v>285.21</v>
       </c>
       <c r="V30" s="3">
-        <v>0.0</v>
+        <v>389.86</v>
       </c>
       <c r="W30" s="3">
-        <v>0.0</v>
+        <v>413.43</v>
       </c>
       <c r="X30" s="3">
-        <v>0.0</v>
+        <v>299.01</v>
       </c>
       <c r="Y30" s="3">
-        <v>0.0</v>
+        <v>295.56</v>
       </c>
       <c r="Z30" s="3">
-        <v>0.0</v>
+        <v>275.44</v>
       </c>
       <c r="AA30" s="3">
-        <v>232.89</v>
+        <v>11253.61</v>
+      </c>
+    </row>
+    <row r="31" spans="1:27">
+      <c r="A31" s="4">
+        <v>11002006</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C31" s="3">
+        <v>163.89</v>
+      </c>
+      <c r="D31" s="3">
+        <v>101.79</v>
+      </c>
+      <c r="E31" s="3">
+        <v>178.84</v>
+      </c>
+      <c r="F31" s="3">
+        <v>239.21</v>
+      </c>
+      <c r="G31" s="3">
+        <v>246.11</v>
+      </c>
+      <c r="H31" s="3">
+        <v>300.73</v>
+      </c>
+      <c r="I31" s="3">
+        <v>543.96</v>
+      </c>
+      <c r="J31" s="3">
+        <v>790.07</v>
+      </c>
+      <c r="K31" s="3">
+        <v>896.43</v>
+      </c>
+      <c r="L31" s="3">
+        <v>886.09</v>
+      </c>
+      <c r="M31" s="3">
+        <v>665.86</v>
+      </c>
+      <c r="N31" s="3">
+        <v>695.19</v>
+      </c>
+      <c r="O31" s="3">
+        <v>865.38</v>
+      </c>
+      <c r="P31" s="3">
+        <v>956.82</v>
+      </c>
+      <c r="Q31" s="3">
+        <v>1039.04</v>
+      </c>
+      <c r="R31" s="3">
+        <v>730.83</v>
+      </c>
+      <c r="S31" s="3">
+        <v>443.33</v>
+      </c>
+      <c r="T31" s="3">
+        <v>426.08</v>
+      </c>
+      <c r="U31" s="3">
+        <v>336.39</v>
+      </c>
+      <c r="V31" s="3">
+        <v>453.11</v>
+      </c>
+      <c r="W31" s="3">
+        <v>478.41</v>
+      </c>
+      <c r="X31" s="3">
+        <v>394.46</v>
+      </c>
+      <c r="Y31" s="3">
+        <v>374.91</v>
+      </c>
+      <c r="Z31" s="3">
+        <v>429.54</v>
+      </c>
+      <c r="AA31" s="3">
+        <v>12636.47</v>
       </c>
     </row>
   </sheetData>
@@ -5544,10 +5713,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:AA30"/>
+  <dimension ref="A1:AA31"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A3" sqref="A3:A30"/>
+      <selection activeCell="A3" sqref="A3:A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5558,7 +5727,7 @@
   <sheetData>
     <row r="1" spans="1:27">
       <c r="A1" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -7994,6 +8163,89 @@
         <v>0.0</v>
       </c>
     </row>
+    <row r="31" spans="1:27">
+      <c r="A31" s="4">
+        <v>11002006</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C31" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="D31" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="E31" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="F31" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="G31" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="H31" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="I31" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="J31" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="K31" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="L31" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="M31" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="N31" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="O31" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="P31" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="Q31" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="R31" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="S31" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="T31" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="U31" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="V31" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="W31" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="X31" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="Y31" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="Z31" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="AA31" s="3">
+        <v>0.0</v>
+      </c>
+    </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
   <mergeCells>
@@ -8018,10 +8270,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:AA30"/>
+  <dimension ref="A1:AA31"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A3" sqref="A3:A30"/>
+      <selection activeCell="A3" sqref="A3:A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8032,7 +8284,7 @@
   <sheetData>
     <row r="1" spans="1:27">
       <c r="A1" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -10468,6 +10720,89 @@
         <v>0.0</v>
       </c>
     </row>
+    <row r="31" spans="1:27">
+      <c r="A31" s="4">
+        <v>11002006</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C31" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="D31" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="E31" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="F31" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="G31" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="H31" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="I31" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="J31" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="K31" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="L31" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="M31" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="N31" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="O31" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="P31" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="Q31" s="3">
+        <v>102.93</v>
+      </c>
+      <c r="R31" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="S31" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="T31" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="U31" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="V31" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="W31" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="X31" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="Y31" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="Z31" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="AA31" s="3">
+        <v>102.93</v>
+      </c>
+    </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
   <mergeCells>
@@ -10492,10 +10827,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:AA30"/>
+  <dimension ref="A1:AA31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A3" sqref="A3:A30"/>
+      <selection activeCell="A3" sqref="A3:A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10506,7 +10841,7 @@
   <sheetData>
     <row r="1" spans="1:27">
       <c r="A1" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -10615,7 +10950,7 @@
         <v>26</v>
       </c>
       <c r="AA2" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:27">
@@ -12873,73 +13208,156 @@
         <v>0.98</v>
       </c>
       <c r="E30" s="3">
-        <v>0</v>
+        <v>0.98</v>
       </c>
       <c r="F30" s="3">
-        <v>0</v>
+        <v>0.98</v>
       </c>
       <c r="G30" s="3">
-        <v>0</v>
+        <v>0.97</v>
       </c>
       <c r="H30" s="3">
-        <v>0</v>
+        <v>0.97</v>
       </c>
       <c r="I30" s="3">
-        <v>0</v>
+        <v>0.94</v>
       </c>
       <c r="J30" s="3">
-        <v>0</v>
+        <v>0.93</v>
       </c>
       <c r="K30" s="3">
-        <v>0</v>
+        <v>0.92</v>
       </c>
       <c r="L30" s="3">
-        <v>0</v>
+        <v>0.91</v>
       </c>
       <c r="M30" s="3">
-        <v>0</v>
+        <v>0.93</v>
       </c>
       <c r="N30" s="3">
-        <v>0</v>
+        <v>0.94</v>
       </c>
       <c r="O30" s="3">
-        <v>0</v>
+        <v>0.91</v>
       </c>
       <c r="P30" s="3">
-        <v>0</v>
+        <v>0.91</v>
       </c>
       <c r="Q30" s="3">
-        <v>0</v>
+        <v>0.93</v>
       </c>
       <c r="R30" s="3">
-        <v>0</v>
+        <v>0.94</v>
       </c>
       <c r="S30" s="3">
-        <v>0</v>
+        <v>0.94</v>
       </c>
       <c r="T30" s="3">
-        <v>0</v>
+        <v>0.94</v>
       </c>
       <c r="U30" s="3">
-        <v>0</v>
+        <v>0.95</v>
       </c>
       <c r="V30" s="3">
-        <v>0</v>
+        <v>0.94</v>
       </c>
       <c r="W30" s="3">
-        <v>0</v>
+        <v>0.93</v>
       </c>
       <c r="X30" s="3">
-        <v>0</v>
+        <v>0.95</v>
       </c>
       <c r="Y30" s="3">
-        <v>0</v>
+        <v>0.95</v>
       </c>
       <c r="Z30" s="3">
-        <v>0</v>
+        <v>0.95</v>
       </c>
       <c r="AA30" s="3">
-        <v>0.08</v>
+        <v>0.94</v>
+      </c>
+    </row>
+    <row r="31" spans="1:27">
+      <c r="A31" s="4">
+        <v>11002006</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C31" s="3">
+        <v>0.97</v>
+      </c>
+      <c r="D31" s="3">
+        <v>0.99</v>
+      </c>
+      <c r="E31" s="3">
+        <v>0.97</v>
+      </c>
+      <c r="F31" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="G31" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="H31" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="I31" s="3">
+        <v>0.94</v>
+      </c>
+      <c r="J31" s="3">
+        <v>0.92</v>
+      </c>
+      <c r="K31" s="3">
+        <v>0.92</v>
+      </c>
+      <c r="L31" s="3">
+        <v>0.92</v>
+      </c>
+      <c r="M31" s="3">
+        <v>0.94</v>
+      </c>
+      <c r="N31" s="3">
+        <v>0.93</v>
+      </c>
+      <c r="O31" s="3">
+        <v>0.92</v>
+      </c>
+      <c r="P31" s="3">
+        <v>0.91</v>
+      </c>
+      <c r="Q31" s="3">
+        <v>0.87</v>
+      </c>
+      <c r="R31" s="3">
+        <v>0.91</v>
+      </c>
+      <c r="S31" s="3">
+        <v>0.93</v>
+      </c>
+      <c r="T31" s="3">
+        <v>0.92</v>
+      </c>
+      <c r="U31" s="3">
+        <v>0.93</v>
+      </c>
+      <c r="V31" s="3">
+        <v>0.92</v>
+      </c>
+      <c r="W31" s="3">
+        <v>0.92</v>
+      </c>
+      <c r="X31" s="3">
+        <v>0.92</v>
+      </c>
+      <c r="Y31" s="3">
+        <v>0.91</v>
+      </c>
+      <c r="Z31" s="3">
+        <v>0.91</v>
+      </c>
+      <c r="AA31" s="3">
+        <v>0.93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>